<commit_message>
updating board review BOM with notes
</commit_message>
<xml_diff>
--- a/BOM/Combined_Board_BOM.xlsx
+++ b/BOM/Combined_Board_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aero\Documents\GitHub\AERO_2021-2022\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B585C8F-1485-48C5-9821-A3EED4670E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01A632F-7EEC-4C64-8E43-1015C572A9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{EA276FB7-F89B-4798-B676-48A298513587}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="279">
   <si>
     <t>Ref</t>
   </si>
@@ -807,9 +807,6 @@
     <t>Q5</t>
   </si>
   <si>
-    <t>Stock</t>
-  </si>
-  <si>
     <t>Board</t>
   </si>
   <si>
@@ -826,6 +823,57 @@
   </si>
   <si>
     <t>RCB</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>In-Stock</t>
+  </si>
+  <si>
+    <t>check value</t>
+  </si>
+  <si>
+    <t>switch footprint</t>
+  </si>
+  <si>
+    <t>Check Footprint and part #</t>
+  </si>
+  <si>
+    <t>check part</t>
+  </si>
+  <si>
+    <t>check stock</t>
+  </si>
+  <si>
+    <t>part number</t>
+  </si>
+  <si>
+    <t>change to 330</t>
+  </si>
+  <si>
+    <t>BUY</t>
+  </si>
+  <si>
+    <t>surface mount?</t>
+  </si>
+  <si>
+    <t>WILLEM!!</t>
+  </si>
+  <si>
+    <t>Find (or buy?)</t>
+  </si>
+  <si>
+    <t>check optoisolator</t>
+  </si>
+  <si>
+    <t>change part</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1243,7 @@
   <dimension ref="A1:H223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,10 +1258,10 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1235,14 +1283,17 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>263</v>
+      </c>
       <c r="B2" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -1252,8 +1303,11 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>265</v>
+      </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1269,14 +1323,17 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>265</v>
+      </c>
       <c r="B4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -1286,6 +1343,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>265</v>
+      </c>
       <c r="B5" t="s">
         <v>258</v>
       </c>
@@ -1293,7 +1353,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -1303,8 +1363,11 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>265</v>
+      </c>
       <c r="B6" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -1320,14 +1383,17 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>265</v>
+      </c>
       <c r="B7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -1337,8 +1403,11 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>265</v>
+      </c>
       <c r="B8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -1354,14 +1423,17 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>265</v>
+      </c>
       <c r="B9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -1371,14 +1443,17 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>263</v>
+      </c>
       <c r="B10" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -1388,8 +1463,11 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>265</v>
+      </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
@@ -1405,14 +1483,17 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>265</v>
+      </c>
       <c r="B12" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -1422,14 +1503,17 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>265</v>
+      </c>
       <c r="B13" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1439,8 +1523,11 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>265</v>
+      </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -1456,8 +1543,11 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>265</v>
+      </c>
       <c r="B15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
@@ -1473,8 +1563,11 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>266</v>
+      </c>
       <c r="B16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
@@ -1489,9 +1582,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>265</v>
+      </c>
       <c r="B17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
@@ -1506,9 +1602,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>265</v>
+      </c>
       <c r="B18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1523,9 +1622,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>266</v>
+      </c>
       <c r="B19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1540,9 +1642,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>265</v>
+      </c>
       <c r="B20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C20" t="s">
         <v>79</v>
@@ -1557,9 +1662,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>265</v>
+      </c>
       <c r="B21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C21" t="s">
         <v>80</v>
@@ -1574,9 +1682,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>265</v>
+      </c>
       <c r="B22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C22" t="s">
         <v>81</v>
@@ -1591,9 +1702,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>265</v>
+      </c>
       <c r="B23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C23" t="s">
         <v>82</v>
@@ -1608,9 +1722,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>267</v>
+      </c>
       <c r="B24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C24" t="s">
         <v>83</v>
@@ -1625,9 +1742,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>265</v>
+      </c>
       <c r="B25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
@@ -1642,9 +1762,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>265</v>
+      </c>
       <c r="B26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
@@ -1659,9 +1782,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>267</v>
+      </c>
       <c r="B27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C27" t="s">
         <v>86</v>
@@ -1676,9 +1802,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>267</v>
+      </c>
       <c r="B28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C28" t="s">
         <v>87</v>
@@ -1693,9 +1822,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>265</v>
+      </c>
       <c r="B29" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C29" t="s">
         <v>88</v>
@@ -1710,9 +1842,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>265</v>
+      </c>
       <c r="B30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C30" t="s">
         <v>90</v>
@@ -1727,9 +1862,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>265</v>
+      </c>
       <c r="B31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C31" t="s">
         <v>91</v>
@@ -1744,9 +1882,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>265</v>
+      </c>
       <c r="B32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
@@ -1761,9 +1902,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>265</v>
+      </c>
       <c r="B33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
@@ -1778,7 +1922,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>265</v>
+      </c>
       <c r="B34" t="s">
         <v>258</v>
       </c>
@@ -1786,7 +1933,7 @@
         <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -1795,15 +1942,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>263</v>
+      </c>
       <c r="B35" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -1812,9 +1962,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>265</v>
+      </c>
       <c r="B36" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
@@ -1829,9 +1982,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>265</v>
+      </c>
       <c r="B37" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C37" t="s">
         <v>16</v>
@@ -1846,9 +2002,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>265</v>
+      </c>
       <c r="B38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
@@ -1863,9 +2022,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>265</v>
+      </c>
       <c r="B39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C39" t="s">
         <v>16</v>
@@ -1880,7 +2042,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>265</v>
+      </c>
       <c r="B40" t="s">
         <v>258</v>
       </c>
@@ -1888,7 +2053,7 @@
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="E40" t="s">
         <v>8</v>
@@ -1897,15 +2062,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>263</v>
+      </c>
       <c r="B41" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
@@ -1914,9 +2082,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>263</v>
+      </c>
       <c r="B42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
@@ -1931,9 +2102,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>265</v>
+      </c>
       <c r="B43" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C43" t="s">
         <v>19</v>
@@ -1948,15 +2122,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>265</v>
+      </c>
       <c r="B44" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C44" t="s">
         <v>19</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E44" t="s">
         <v>8</v>
@@ -1965,15 +2142,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>263</v>
+      </c>
       <c r="B45" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C45" t="s">
         <v>19</v>
       </c>
       <c r="D45" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
@@ -1982,9 +2162,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>265</v>
+      </c>
       <c r="B46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C46" t="s">
         <v>20</v>
@@ -1999,9 +2182,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>265</v>
+      </c>
       <c r="B47" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C47" t="s">
         <v>20</v>
@@ -2016,7 +2202,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>265</v>
+      </c>
       <c r="B48" t="s">
         <v>258</v>
       </c>
@@ -2024,7 +2213,7 @@
         <v>21</v>
       </c>
       <c r="D48" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
@@ -2033,15 +2222,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>265</v>
+      </c>
       <c r="B49" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C49" t="s">
         <v>21</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E49" t="s">
         <v>8</v>
@@ -2050,9 +2242,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>265</v>
+      </c>
       <c r="B50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C50" t="s">
         <v>21</v>
@@ -2067,9 +2262,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>268</v>
+      </c>
       <c r="B51" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C51" t="s">
         <v>27</v>
@@ -2084,9 +2282,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>268</v>
+      </c>
       <c r="B52" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C52" t="s">
         <v>27</v>
@@ -2101,26 +2302,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>268</v>
+      </c>
       <c r="B53" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C53" t="s">
         <v>27</v>
       </c>
       <c r="D53" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E53" t="s">
-        <v>32</v>
+        <v>222</v>
       </c>
       <c r="F53" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>265</v>
+      </c>
       <c r="B54" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C54" t="s">
         <v>27</v>
@@ -2129,15 +2336,18 @@
         <v>31</v>
       </c>
       <c r="E54" t="s">
-        <v>186</v>
+        <v>32</v>
       </c>
       <c r="F54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>265</v>
+      </c>
       <c r="B55" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C55" t="s">
         <v>27</v>
@@ -2152,26 +2362,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>265</v>
+      </c>
       <c r="B56" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C56" t="s">
         <v>27</v>
       </c>
       <c r="D56" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E56" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="F56" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>265</v>
+      </c>
       <c r="B57" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C57" t="s">
         <v>30</v>
@@ -2186,9 +2402,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>265</v>
+      </c>
       <c r="B58" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C58" t="s">
         <v>30</v>
@@ -2203,9 +2422,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>265</v>
+      </c>
       <c r="B59" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C59" t="s">
         <v>30</v>
@@ -2220,9 +2442,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>265</v>
+      </c>
       <c r="B60" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C60" t="s">
         <v>30</v>
@@ -2237,9 +2462,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>265</v>
+      </c>
       <c r="B61" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C61" t="s">
         <v>187</v>
@@ -2254,9 +2482,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>265</v>
+      </c>
       <c r="B62" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C62" t="s">
         <v>187</v>
@@ -2271,9 +2502,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>269</v>
+      </c>
       <c r="B63" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C63" t="s">
         <v>187</v>
@@ -2288,9 +2522,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>267</v>
+      </c>
       <c r="B64" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C64" t="s">
         <v>191</v>
@@ -2305,9 +2542,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>267</v>
+      </c>
       <c r="B65" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C65" t="s">
         <v>191</v>
@@ -2322,9 +2562,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>267</v>
+      </c>
       <c r="B66" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C66" t="s">
         <v>191</v>
@@ -2339,7 +2582,10 @@
         <v>226</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>267</v>
+      </c>
       <c r="B67" t="s">
         <v>261</v>
       </c>
@@ -2347,18 +2593,21 @@
         <v>192</v>
       </c>
       <c r="D67" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E67" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="F67" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>269</v>
+      </c>
       <c r="B68" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C68" t="s">
         <v>192</v>
@@ -2373,43 +2622,52 @@
         <v>195</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>269</v>
+      </c>
       <c r="B69" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C69" t="s">
         <v>192</v>
       </c>
       <c r="D69" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E69" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="F69" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>265</v>
+      </c>
       <c r="B70" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C70" t="s">
         <v>93</v>
       </c>
       <c r="D70" t="s">
-        <v>94</v>
+        <v>196</v>
       </c>
       <c r="E70" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
       <c r="F70" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>265</v>
+      </c>
       <c r="B71" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C71" t="s">
         <v>93</v>
@@ -2424,26 +2682,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>265</v>
+      </c>
       <c r="B72" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C72" t="s">
         <v>93</v>
       </c>
       <c r="D72" t="s">
-        <v>196</v>
+        <v>94</v>
       </c>
       <c r="E72" t="s">
-        <v>197</v>
+        <v>95</v>
       </c>
       <c r="F72" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>265</v>
+      </c>
       <c r="B73" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C73" t="s">
         <v>93</v>
@@ -2458,9 +2722,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>265</v>
+      </c>
       <c r="B74" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C74" t="s">
         <v>236</v>
@@ -2475,9 +2742,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>265</v>
+      </c>
       <c r="B75" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C75" t="s">
         <v>238</v>
@@ -2492,26 +2762,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>265</v>
+      </c>
       <c r="B76" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C76" t="s">
         <v>96</v>
       </c>
       <c r="D76" t="s">
-        <v>94</v>
+        <v>227</v>
       </c>
       <c r="E76" t="s">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="F76" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>265</v>
+      </c>
       <c r="B77" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C77" t="s">
         <v>96</v>
@@ -2526,9 +2802,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>265</v>
+      </c>
       <c r="B78" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C78" t="s">
         <v>96</v>
@@ -2543,24 +2822,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>265</v>
+      </c>
       <c r="B79" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C79" t="s">
         <v>96</v>
       </c>
       <c r="D79" t="s">
-        <v>227</v>
+        <v>94</v>
       </c>
       <c r="E79" t="s">
-        <v>200</v>
+        <v>95</v>
       </c>
       <c r="F79" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>265</v>
+      </c>
       <c r="B80" t="s">
         <v>261</v>
       </c>
@@ -2568,7 +2853,7 @@
         <v>198</v>
       </c>
       <c r="D80" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="E80" t="s">
         <v>200</v>
@@ -2577,9 +2862,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>265</v>
+      </c>
       <c r="B81" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C81" t="s">
         <v>198</v>
@@ -2594,15 +2882,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>265</v>
+      </c>
       <c r="B82" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C82" t="s">
         <v>198</v>
       </c>
       <c r="D82" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="E82" t="s">
         <v>200</v>
@@ -2611,9 +2902,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>265</v>
+      </c>
       <c r="B83" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C83" t="s">
         <v>229</v>
@@ -2628,9 +2922,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>265</v>
+      </c>
       <c r="B84" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C84" t="s">
         <v>230</v>
@@ -2645,9 +2942,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>265</v>
+      </c>
       <c r="B85" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C85" t="s">
         <v>231</v>
@@ -2662,9 +2962,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>265</v>
+      </c>
       <c r="B86" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C86" t="s">
         <v>232</v>
@@ -2679,9 +2982,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>265</v>
+      </c>
       <c r="B87" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C87" t="s">
         <v>234</v>
@@ -2696,9 +3002,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>265</v>
+      </c>
       <c r="B88" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C88" t="s">
         <v>235</v>
@@ -2713,9 +3022,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>265</v>
+      </c>
       <c r="B89" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C89" t="s">
         <v>97</v>
@@ -2730,9 +3042,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>265</v>
+      </c>
       <c r="B90" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C90" t="s">
         <v>97</v>
@@ -2747,9 +3062,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>265</v>
+      </c>
       <c r="B91" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C91" t="s">
         <v>97</v>
@@ -2764,9 +3082,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>265</v>
+      </c>
       <c r="B92" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C92" t="s">
         <v>100</v>
@@ -2781,9 +3102,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>265</v>
+      </c>
       <c r="B93" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C93" t="s">
         <v>100</v>
@@ -2798,9 +3122,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>265</v>
+      </c>
       <c r="B94" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C94" t="s">
         <v>100</v>
@@ -2815,9 +3142,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>265</v>
+      </c>
       <c r="B95" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C95" t="s">
         <v>101</v>
@@ -2832,9 +3162,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>265</v>
+      </c>
       <c r="B96" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C96" t="s">
         <v>102</v>
@@ -2849,9 +3182,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>265</v>
+      </c>
       <c r="B97" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C97" t="s">
         <v>33</v>
@@ -2866,24 +3202,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>270</v>
+      </c>
       <c r="B98" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C98" t="s">
         <v>33</v>
       </c>
       <c r="D98" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E98" t="s">
-        <v>44</v>
+        <v>201</v>
       </c>
       <c r="F98" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>270</v>
+      </c>
       <c r="B99" t="s">
         <v>260</v>
       </c>
@@ -2891,52 +3233,61 @@
         <v>33</v>
       </c>
       <c r="D99" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E99" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="F99" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>270</v>
+      </c>
       <c r="B100" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C100" t="s">
         <v>33</v>
       </c>
       <c r="D100" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E100" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="F100" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>270</v>
+      </c>
       <c r="B101" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C101" t="s">
         <v>33</v>
       </c>
       <c r="D101" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E101" t="s">
-        <v>201</v>
+        <v>44</v>
       </c>
       <c r="F101" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>270</v>
+      </c>
       <c r="B102" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C102" t="s">
         <v>33</v>
@@ -2951,9 +3302,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>270</v>
+      </c>
       <c r="B103" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C103" t="s">
         <v>114</v>
@@ -2968,9 +3322,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>270</v>
+      </c>
       <c r="B104" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C104" t="s">
         <v>116</v>
@@ -2985,43 +3342,52 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>270</v>
+      </c>
       <c r="B105" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C105" t="s">
         <v>36</v>
       </c>
       <c r="D105" t="s">
-        <v>37</v>
+        <v>202</v>
       </c>
       <c r="E105" t="s">
-        <v>38</v>
+        <v>203</v>
       </c>
       <c r="F105" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>270</v>
+      </c>
       <c r="B106" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C106" t="s">
         <v>36</v>
       </c>
       <c r="D106" t="s">
-        <v>103</v>
+        <v>202</v>
       </c>
       <c r="E106" t="s">
-        <v>35</v>
+        <v>203</v>
       </c>
       <c r="F106" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>270</v>
+      </c>
       <c r="B107" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C107" t="s">
         <v>36</v>
@@ -3036,24 +3402,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>270</v>
+      </c>
       <c r="B108" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C108" t="s">
         <v>36</v>
       </c>
       <c r="D108" t="s">
-        <v>202</v>
+        <v>37</v>
       </c>
       <c r="E108" t="s">
-        <v>203</v>
+        <v>38</v>
       </c>
       <c r="F108" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>270</v>
+      </c>
       <c r="B109" t="s">
         <v>261</v>
       </c>
@@ -3061,58 +3433,67 @@
         <v>36</v>
       </c>
       <c r="D109" t="s">
-        <v>202</v>
+        <v>37</v>
       </c>
       <c r="E109" t="s">
-        <v>203</v>
+        <v>38</v>
       </c>
       <c r="F109" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>265</v>
+      </c>
       <c r="B110" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C110" t="s">
         <v>36</v>
       </c>
       <c r="D110" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="E110" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F110" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>270</v>
+      </c>
       <c r="B111" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C111" t="s">
         <v>39</v>
       </c>
       <c r="D111" t="s">
-        <v>40</v>
+        <v>204</v>
       </c>
       <c r="E111" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="F111" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>270</v>
+      </c>
       <c r="B112" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C112" t="s">
         <v>39</v>
       </c>
       <c r="D112" t="s">
-        <v>104</v>
+        <v>204</v>
       </c>
       <c r="E112" t="s">
         <v>105</v>
@@ -3121,24 +3502,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>270</v>
+      </c>
       <c r="B113" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C113" t="s">
         <v>39</v>
       </c>
       <c r="D113" t="s">
-        <v>204</v>
+        <v>40</v>
       </c>
       <c r="E113" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="F113" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>270</v>
+      </c>
       <c r="B114" t="s">
         <v>261</v>
       </c>
@@ -3146,58 +3533,67 @@
         <v>39</v>
       </c>
       <c r="D114" t="s">
-        <v>204</v>
+        <v>40</v>
       </c>
       <c r="E114" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="F114" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>270</v>
+      </c>
       <c r="B115" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C115" t="s">
         <v>39</v>
       </c>
       <c r="D115" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="E115" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="F115" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>270</v>
+      </c>
       <c r="B116" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C116" t="s">
         <v>42</v>
       </c>
       <c r="D116" t="s">
-        <v>43</v>
+        <v>204</v>
       </c>
       <c r="E116" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="F116" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>270</v>
+      </c>
       <c r="B117" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C117" t="s">
         <v>42</v>
       </c>
       <c r="D117" t="s">
-        <v>106</v>
+        <v>204</v>
       </c>
       <c r="E117" t="s">
         <v>105</v>
@@ -3206,7 +3602,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>270</v>
+      </c>
       <c r="B118" t="s">
         <v>261</v>
       </c>
@@ -3214,84 +3613,99 @@
         <v>42</v>
       </c>
       <c r="D118" t="s">
-        <v>204</v>
+        <v>109</v>
       </c>
       <c r="E118" t="s">
-        <v>105</v>
+        <v>240</v>
       </c>
       <c r="F118" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>270</v>
+      </c>
       <c r="B119" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C119" t="s">
         <v>42</v>
       </c>
       <c r="D119" t="s">
-        <v>204</v>
+        <v>43</v>
       </c>
       <c r="E119" t="s">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="F119" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>270</v>
+      </c>
       <c r="B120" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C120" t="s">
         <v>42</v>
       </c>
       <c r="D120" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E120" t="s">
-        <v>240</v>
+        <v>105</v>
       </c>
       <c r="F120" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>270</v>
+      </c>
       <c r="B121" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C121" t="s">
         <v>45</v>
       </c>
       <c r="D121" t="s">
-        <v>46</v>
+        <v>204</v>
       </c>
       <c r="E121" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="F121" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>270</v>
+      </c>
       <c r="B122" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C122" t="s">
         <v>45</v>
       </c>
       <c r="D122" t="s">
-        <v>104</v>
+        <v>204</v>
       </c>
       <c r="E122" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F122" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>270</v>
+      </c>
       <c r="B123" t="s">
         <v>261</v>
       </c>
@@ -3299,84 +3713,99 @@
         <v>45</v>
       </c>
       <c r="D123" t="s">
-        <v>204</v>
+        <v>109</v>
       </c>
       <c r="E123" t="s">
-        <v>105</v>
+        <v>240</v>
       </c>
       <c r="F123" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>270</v>
+      </c>
       <c r="B124" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C124" t="s">
         <v>45</v>
       </c>
       <c r="D124" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="E124" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="F124" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>270</v>
+      </c>
       <c r="B125" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C125" t="s">
         <v>45</v>
       </c>
       <c r="D125" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E125" t="s">
-        <v>240</v>
+        <v>107</v>
       </c>
       <c r="F125" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>270</v>
+      </c>
       <c r="B126" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C126" t="s">
         <v>48</v>
       </c>
       <c r="D126" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="E126" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F126" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>270</v>
+      </c>
       <c r="B127" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C127" t="s">
         <v>48</v>
       </c>
       <c r="D127" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E127" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F127" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>270</v>
+      </c>
       <c r="B128" t="s">
         <v>261</v>
       </c>
@@ -3384,52 +3813,61 @@
         <v>48</v>
       </c>
       <c r="D128" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
       <c r="E128" t="s">
-        <v>110</v>
+        <v>35</v>
       </c>
       <c r="F128" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>270</v>
+      </c>
       <c r="B129" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C129" t="s">
         <v>48</v>
       </c>
       <c r="D129" t="s">
-        <v>109</v>
+        <v>37</v>
       </c>
       <c r="E129" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="F129" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>270</v>
+      </c>
       <c r="B130" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C130" t="s">
         <v>48</v>
       </c>
       <c r="D130" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="E130" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="F130" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>270</v>
+      </c>
       <c r="B131" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C131" t="s">
         <v>108</v>
@@ -3444,9 +3882,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>270</v>
+      </c>
       <c r="B132" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C132" t="s">
         <v>111</v>
@@ -3461,9 +3902,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>270</v>
+      </c>
       <c r="B133" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C133" t="s">
         <v>112</v>
@@ -3478,9 +3922,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>270</v>
+      </c>
       <c r="B134" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C134" t="s">
         <v>112</v>
@@ -3495,9 +3942,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>270</v>
+      </c>
       <c r="B135" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C135" t="s">
         <v>112</v>
@@ -3512,9 +3962,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>265</v>
+      </c>
       <c r="B136" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C136" t="s">
         <v>207</v>
@@ -3529,9 +3982,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>265</v>
+      </c>
       <c r="B137" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C137" t="s">
         <v>207</v>
@@ -3546,9 +4002,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>265</v>
+      </c>
       <c r="B138" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C138" t="s">
         <v>207</v>
@@ -3563,9 +4022,12 @@
         <v>243</v>
       </c>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>265</v>
+      </c>
       <c r="B139" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C139" t="s">
         <v>211</v>
@@ -3580,9 +4042,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>265</v>
+      </c>
       <c r="B140" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C140" t="s">
         <v>211</v>
@@ -3597,9 +4062,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>265</v>
+      </c>
       <c r="B141" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C141" t="s">
         <v>211</v>
@@ -3614,9 +4082,12 @@
         <v>246</v>
       </c>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>265</v>
+      </c>
       <c r="B142" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C142" t="s">
         <v>214</v>
@@ -3631,9 +4102,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>265</v>
+      </c>
       <c r="B143" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C143" t="s">
         <v>214</v>
@@ -3648,9 +4122,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>265</v>
+      </c>
       <c r="B144" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C144" t="s">
         <v>214</v>
@@ -3665,9 +4142,12 @@
         <v>246</v>
       </c>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>267</v>
+      </c>
       <c r="B145" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C145" t="s">
         <v>117</v>
@@ -3682,9 +4162,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>267</v>
+      </c>
       <c r="B146" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C146" t="s">
         <v>120</v>
@@ -3699,60 +4182,72 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>265</v>
+      </c>
       <c r="B147" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C147" t="s">
         <v>122</v>
       </c>
       <c r="D147" t="s">
-        <v>123</v>
+        <v>247</v>
       </c>
       <c r="E147" t="s">
-        <v>124</v>
+        <v>194</v>
       </c>
       <c r="F147" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>265</v>
+      </c>
       <c r="B148" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C148" t="s">
         <v>122</v>
       </c>
       <c r="D148" t="s">
-        <v>247</v>
+        <v>123</v>
       </c>
       <c r="E148" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="F148" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>265</v>
+      </c>
       <c r="B149" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C149" t="s">
         <v>126</v>
       </c>
       <c r="D149" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="E149" t="s">
-        <v>124</v>
+        <v>194</v>
       </c>
       <c r="F149" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>265</v>
+      </c>
       <c r="B150" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C150" t="s">
         <v>126</v>
@@ -3767,9 +4262,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>265</v>
+      </c>
       <c r="B151" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C151" t="s">
         <v>126</v>
@@ -3784,26 +4282,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>265</v>
+      </c>
       <c r="B152" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C152" t="s">
         <v>126</v>
       </c>
       <c r="D152" t="s">
-        <v>249</v>
+        <v>123</v>
       </c>
       <c r="E152" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="F152" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>271</v>
+      </c>
       <c r="B153" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C153" t="s">
         <v>251</v>
@@ -3818,9 +4322,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>271</v>
+      </c>
       <c r="B154" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C154" t="s">
         <v>254</v>
@@ -3835,9 +4342,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>271</v>
+      </c>
       <c r="B155" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C155" t="s">
         <v>255</v>
@@ -3852,9 +4362,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>272</v>
+      </c>
       <c r="B156" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C156" t="s">
         <v>49</v>
@@ -3869,26 +4382,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>272</v>
+      </c>
       <c r="B157" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C157" t="s">
         <v>49</v>
       </c>
-      <c r="D157" t="s">
-        <v>127</v>
+      <c r="D157">
+        <v>220</v>
       </c>
       <c r="E157" t="s">
-        <v>128</v>
+        <v>50</v>
       </c>
       <c r="F157" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>266</v>
+      </c>
       <c r="B158" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C158" t="s">
         <v>49</v>
@@ -3897,15 +4416,18 @@
         <v>127</v>
       </c>
       <c r="E158" t="s">
-        <v>216</v>
+        <v>128</v>
       </c>
       <c r="F158" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>266</v>
+      </c>
       <c r="B159" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C159" t="s">
         <v>49</v>
@@ -3920,26 +4442,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>266</v>
+      </c>
       <c r="B160" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C160" t="s">
         <v>49</v>
       </c>
-      <c r="D160">
-        <v>220</v>
+      <c r="D160" t="s">
+        <v>127</v>
       </c>
       <c r="E160" t="s">
-        <v>50</v>
+        <v>216</v>
       </c>
       <c r="F160" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>266</v>
+      </c>
       <c r="B161" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C161" t="s">
         <v>139</v>
@@ -3954,9 +4482,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>265</v>
+      </c>
       <c r="B162" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C162" t="s">
         <v>140</v>
@@ -3971,9 +4502,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>265</v>
+      </c>
       <c r="B163" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C163" t="s">
         <v>141</v>
@@ -3988,9 +4522,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>265</v>
+      </c>
       <c r="B164" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C164" t="s">
         <v>142</v>
@@ -4005,9 +4542,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>266</v>
+      </c>
       <c r="B165" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C165" t="s">
         <v>143</v>
@@ -4022,9 +4562,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>266</v>
+      </c>
       <c r="B166" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C166" t="s">
         <v>145</v>
@@ -4039,9 +4582,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>265</v>
+      </c>
       <c r="B167" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C167" t="s">
         <v>147</v>
@@ -4056,9 +4602,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>265</v>
+      </c>
       <c r="B168" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C168" t="s">
         <v>148</v>
@@ -4073,9 +4622,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>265</v>
+      </c>
       <c r="B169" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C169" t="s">
         <v>149</v>
@@ -4090,15 +4642,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>265</v>
+      </c>
       <c r="B170" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C170" t="s">
         <v>129</v>
       </c>
-      <c r="D170" t="s">
-        <v>130</v>
+      <c r="D170">
+        <v>120</v>
       </c>
       <c r="E170" t="s">
         <v>50</v>
@@ -4107,9 +4662,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>265</v>
+      </c>
       <c r="B171" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C171" t="s">
         <v>129</v>
@@ -4124,15 +4682,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>265</v>
+      </c>
       <c r="B172" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C172" t="s">
         <v>129</v>
       </c>
-      <c r="D172">
-        <v>120</v>
+      <c r="D172" t="s">
+        <v>130</v>
       </c>
       <c r="E172" t="s">
         <v>50</v>
@@ -4141,9 +4702,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>265</v>
+      </c>
       <c r="B173" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C173" t="s">
         <v>129</v>
@@ -4158,9 +4722,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>266</v>
+      </c>
       <c r="B174" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C174" t="s">
         <v>150</v>
@@ -4175,9 +4742,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>262</v>
+      </c>
       <c r="B175" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C175" t="s">
         <v>131</v>
@@ -4192,9 +4762,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>262</v>
+      </c>
       <c r="B176" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C176" t="s">
         <v>131</v>
@@ -4209,26 +4782,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>266</v>
+      </c>
       <c r="B177" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C177" t="s">
         <v>133</v>
       </c>
       <c r="D177" t="s">
-        <v>134</v>
+        <v>217</v>
       </c>
       <c r="E177" t="s">
-        <v>50</v>
+        <v>218</v>
       </c>
       <c r="F177" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>266</v>
+      </c>
       <c r="B178" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C178" t="s">
         <v>133</v>
@@ -4243,26 +4822,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>273</v>
+      </c>
       <c r="B179" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C179" t="s">
         <v>133</v>
       </c>
       <c r="D179" t="s">
-        <v>217</v>
+        <v>134</v>
       </c>
       <c r="E179" t="s">
-        <v>218</v>
+        <v>50</v>
       </c>
       <c r="F179" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>265</v>
+      </c>
       <c r="B180" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C180" t="s">
         <v>135</v>
@@ -4277,9 +4862,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>265</v>
+      </c>
       <c r="B181" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C181" t="s">
         <v>135</v>
@@ -4294,9 +4882,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>265</v>
+      </c>
       <c r="B182" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C182" t="s">
         <v>135</v>
@@ -4311,9 +4902,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>265</v>
+      </c>
       <c r="B183" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C183" t="s">
         <v>135</v>
@@ -4328,43 +4922,52 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>273</v>
+      </c>
       <c r="B184" t="s">
         <v>258</v>
       </c>
       <c r="C184" t="s">
         <v>51</v>
       </c>
-      <c r="D184" t="s">
-        <v>52</v>
+      <c r="D184">
+        <v>0.75</v>
       </c>
       <c r="E184" t="s">
-        <v>50</v>
+        <v>136</v>
       </c>
       <c r="F184" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>265</v>
+      </c>
       <c r="B185" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C185" t="s">
         <v>51</v>
       </c>
       <c r="D185">
-        <v>0.75</v>
+        <v>120</v>
       </c>
       <c r="E185" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="F185" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>265</v>
+      </c>
       <c r="B186" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C186" t="s">
         <v>51</v>
@@ -4379,9 +4982,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>265</v>
+      </c>
       <c r="B187" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C187" t="s">
         <v>51</v>
@@ -4396,15 +5002,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>266</v>
+      </c>
       <c r="B188" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C188" t="s">
         <v>51</v>
       </c>
-      <c r="D188">
-        <v>120</v>
+      <c r="D188" t="s">
+        <v>52</v>
       </c>
       <c r="E188" t="s">
         <v>50</v>
@@ -4413,15 +5022,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>272</v>
+      </c>
       <c r="B189" t="s">
         <v>258</v>
       </c>
       <c r="C189" t="s">
         <v>53</v>
       </c>
-      <c r="D189" t="s">
-        <v>54</v>
+      <c r="D189">
+        <v>220</v>
       </c>
       <c r="E189" t="s">
         <v>50</v>
@@ -4430,15 +5042,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>265</v>
+      </c>
       <c r="B190" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C190" t="s">
         <v>53</v>
       </c>
-      <c r="D190">
-        <v>220</v>
+      <c r="D190" t="s">
+        <v>130</v>
       </c>
       <c r="E190" t="s">
         <v>50</v>
@@ -4447,26 +5062,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>265</v>
+      </c>
       <c r="B191" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C191" t="s">
         <v>53</v>
       </c>
       <c r="D191" t="s">
-        <v>217</v>
+        <v>54</v>
       </c>
       <c r="E191" t="s">
-        <v>218</v>
+        <v>50</v>
       </c>
       <c r="F191" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>266</v>
+      </c>
       <c r="B192" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C192" t="s">
         <v>53</v>
@@ -4481,26 +5102,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>266</v>
+      </c>
       <c r="B193" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C193" t="s">
         <v>53</v>
       </c>
       <c r="D193" t="s">
-        <v>130</v>
+        <v>217</v>
       </c>
       <c r="E193" t="s">
-        <v>50</v>
+        <v>218</v>
       </c>
       <c r="F193" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>265</v>
+      </c>
       <c r="B194" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C194" t="s">
         <v>55</v>
@@ -4515,9 +5142,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>266</v>
+      </c>
       <c r="B195" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C195" t="s">
         <v>55</v>
@@ -4532,9 +5162,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>266</v>
+      </c>
       <c r="B196" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C196" t="s">
         <v>137</v>
@@ -4549,9 +5182,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>265</v>
+      </c>
       <c r="B197" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C197" t="s">
         <v>56</v>
@@ -4566,9 +5202,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>274</v>
+      </c>
       <c r="B198" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C198" t="s">
         <v>151</v>
@@ -4581,9 +5220,12 @@
       </c>
       <c r="F198"/>
     </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>265</v>
+      </c>
       <c r="B199" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C199" t="s">
         <v>151</v>
@@ -4596,9 +5238,12 @@
       </c>
       <c r="F199"/>
     </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>265</v>
+      </c>
       <c r="B200" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C200" t="s">
         <v>175</v>
@@ -4611,9 +5256,12 @@
       </c>
       <c r="F200"/>
     </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>274</v>
+      </c>
       <c r="B201" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C201" t="s">
         <v>176</v>
@@ -4628,9 +5276,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>274</v>
+      </c>
       <c r="B202" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C202" t="s">
         <v>179</v>
@@ -4645,9 +5296,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>274</v>
+      </c>
       <c r="B203" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C203" t="s">
         <v>180</v>
@@ -4662,9 +5316,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>274</v>
+      </c>
       <c r="B204" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C204" t="s">
         <v>183</v>
@@ -4679,9 +5336,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>275</v>
+      </c>
       <c r="B205" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C205" t="s">
         <v>59</v>
@@ -4696,9 +5356,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="206" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C206" t="s">
         <v>59</v>
@@ -4713,9 +5373,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>265</v>
+      </c>
       <c r="B207" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C207" t="s">
         <v>63</v>
@@ -4730,41 +5393,50 @@
         <v>66</v>
       </c>
     </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>265</v>
+      </c>
       <c r="B208" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C208" t="s">
         <v>63</v>
       </c>
       <c r="D208" t="s">
-        <v>154</v>
+        <v>64</v>
       </c>
       <c r="E208" t="s">
-        <v>155</v>
+        <v>65</v>
       </c>
       <c r="F208" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>265</v>
+      </c>
       <c r="B209" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C209" t="s">
         <v>63</v>
       </c>
       <c r="D209" t="s">
-        <v>64</v>
+        <v>154</v>
       </c>
       <c r="E209" t="s">
-        <v>65</v>
+        <v>155</v>
       </c>
       <c r="F209" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>265</v>
+      </c>
       <c r="B210" t="s">
         <v>258</v>
       </c>
@@ -4772,35 +5444,41 @@
         <v>67</v>
       </c>
       <c r="D210" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
       <c r="E210" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F210" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>265</v>
+      </c>
       <c r="B211" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C211" t="s">
         <v>67</v>
       </c>
       <c r="D211" t="s">
-        <v>157</v>
+        <v>68</v>
       </c>
       <c r="E211" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F211" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>265</v>
+      </c>
       <c r="B212" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C212" t="s">
         <v>67</v>
@@ -4815,7 +5493,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>265</v>
+      </c>
       <c r="B213" t="s">
         <v>258</v>
       </c>
@@ -4823,35 +5504,41 @@
         <v>71</v>
       </c>
       <c r="D213" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E213" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F213" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>276</v>
+      </c>
       <c r="B214" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C214" t="s">
         <v>71</v>
       </c>
       <c r="D214" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E214" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F214" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>276</v>
+      </c>
       <c r="B215" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C215" t="s">
         <v>71</v>
@@ -4866,9 +5553,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="216" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>275</v>
+      </c>
       <c r="B216" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C216" t="s">
         <v>159</v>
@@ -4883,9 +5573,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>276</v>
+      </c>
       <c r="B217" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C217" t="s">
         <v>161</v>
@@ -4900,9 +5593,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>265</v>
+      </c>
       <c r="B218" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C218" t="s">
         <v>162</v>
@@ -4915,9 +5611,12 @@
       </c>
       <c r="F218"/>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>265</v>
+      </c>
       <c r="B219" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C219" t="s">
         <v>165</v>
@@ -4932,9 +5631,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>277</v>
+      </c>
       <c r="B220" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C220" t="s">
         <v>166</v>
@@ -4949,9 +5651,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>278</v>
+      </c>
       <c r="B221" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C221" t="s">
         <v>75</v>
@@ -4966,9 +5671,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>278</v>
+      </c>
       <c r="B222" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C222" t="s">
         <v>75</v>
@@ -4983,9 +5691,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>278</v>
+      </c>
       <c r="B223" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C223" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
Major Review and Part Update
updating footprints, component values, layouts
</commit_message>
<xml_diff>
--- a/BOM/Combined_Board_BOM.xlsx
+++ b/BOM/Combined_Board_BOM.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aero\Documents\GitHub\AERO_2021-2022\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01A632F-7EEC-4C64-8E43-1015C572A9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF552DD-A066-4D26-BA93-8DD2E9D51543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{EA276FB7-F89B-4798-B676-48A298513587}"/>
+    <workbookView xWindow="-43320" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{EA276FB7-F89B-4798-B676-48A298513587}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$223</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="278">
   <si>
     <t>Ref</t>
   </si>
@@ -828,9 +828,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>remove</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -843,9 +840,6 @@
     <t>switch footprint</t>
   </si>
   <si>
-    <t>Check Footprint and part #</t>
-  </si>
-  <si>
     <t>check part</t>
   </si>
   <si>
@@ -855,9 +849,6 @@
     <t>part number</t>
   </si>
   <si>
-    <t>change to 330</t>
-  </si>
-  <si>
     <t>BUY</t>
   </si>
   <si>
@@ -873,7 +864,13 @@
     <t>check optoisolator</t>
   </si>
   <si>
-    <t>change part</t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Doen</t>
   </si>
 </sst>
 </file>
@@ -1242,12 +1239,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB690B54-ADEF-4B77-BFF1-9B7541870C3F}">
   <dimension ref="A1:H223"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="64.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1258,7 +1256,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>256</v>
@@ -1284,7 +1282,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
         <v>261</v>
@@ -1304,7 +1302,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B3" t="s">
         <v>257</v>
@@ -1324,7 +1322,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B4" t="s">
         <v>258</v>
@@ -1344,7 +1342,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B5" t="s">
         <v>258</v>
@@ -1364,7 +1362,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
         <v>261</v>
@@ -1384,7 +1382,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B7" t="s">
         <v>257</v>
@@ -1404,7 +1402,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B8" t="s">
         <v>257</v>
@@ -1424,7 +1422,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B9" t="s">
         <v>261</v>
@@ -1444,7 +1442,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="B10" t="s">
         <v>258</v>
@@ -1464,7 +1462,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B11" t="s">
         <v>257</v>
@@ -1484,7 +1482,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B12" t="s">
         <v>261</v>
@@ -1504,7 +1502,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B13" t="s">
         <v>258</v>
@@ -1524,7 +1522,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B14" t="s">
         <v>257</v>
@@ -1544,7 +1542,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B15" t="s">
         <v>258</v>
@@ -1564,7 +1562,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B16" t="s">
         <v>261</v>
@@ -1584,7 +1582,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B17" t="s">
         <v>257</v>
@@ -1604,7 +1602,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B18" t="s">
         <v>258</v>
@@ -1624,7 +1622,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B19" t="s">
         <v>261</v>
@@ -1644,7 +1642,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B20" t="s">
         <v>258</v>
@@ -1664,7 +1662,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B21" t="s">
         <v>258</v>
@@ -1684,7 +1682,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B22" t="s">
         <v>258</v>
@@ -1704,7 +1702,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B23" t="s">
         <v>258</v>
@@ -1724,7 +1722,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B24" t="s">
         <v>258</v>
@@ -1744,7 +1742,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B25" t="s">
         <v>257</v>
@@ -1764,7 +1762,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B26" t="s">
         <v>261</v>
@@ -1784,7 +1782,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B27" t="s">
         <v>258</v>
@@ -1804,7 +1802,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B28" t="s">
         <v>258</v>
@@ -1824,7 +1822,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B29" t="s">
         <v>258</v>
@@ -1844,7 +1842,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B30" t="s">
         <v>258</v>
@@ -1864,7 +1862,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B31" t="s">
         <v>258</v>
@@ -1884,7 +1882,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s">
         <v>257</v>
@@ -1904,7 +1902,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B33" t="s">
         <v>261</v>
@@ -1924,7 +1922,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B34" t="s">
         <v>258</v>
@@ -1944,7 +1942,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="B35" t="s">
         <v>257</v>
@@ -1964,7 +1962,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B36" t="s">
         <v>261</v>
@@ -1984,7 +1982,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B37" t="s">
         <v>257</v>
@@ -2004,7 +2002,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B38" t="s">
         <v>258</v>
@@ -2024,7 +2022,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B39" t="s">
         <v>261</v>
@@ -2044,7 +2042,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B40" t="s">
         <v>258</v>
@@ -2064,7 +2062,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="B41" t="s">
         <v>257</v>
@@ -2084,7 +2082,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="B42" t="s">
         <v>261</v>
@@ -2104,7 +2102,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B43" t="s">
         <v>257</v>
@@ -2124,7 +2122,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B44" t="s">
         <v>261</v>
@@ -2144,7 +2142,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="B45" t="s">
         <v>258</v>
@@ -2164,7 +2162,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B46" t="s">
         <v>257</v>
@@ -2184,7 +2182,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B47" t="s">
         <v>261</v>
@@ -2204,7 +2202,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B48" t="s">
         <v>258</v>
@@ -2224,7 +2222,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B49" t="s">
         <v>257</v>
@@ -2244,7 +2242,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B50" t="s">
         <v>261</v>
@@ -2264,7 +2262,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="B51" t="s">
         <v>257</v>
@@ -2284,7 +2282,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B52" t="s">
         <v>258</v>
@@ -2304,7 +2302,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B53" t="s">
         <v>261</v>
@@ -2324,7 +2322,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B54" t="s">
         <v>259</v>
@@ -2344,7 +2342,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B55" t="s">
         <v>260</v>
@@ -2364,7 +2362,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B56" t="s">
         <v>260</v>
@@ -2384,7 +2382,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B57" t="s">
         <v>257</v>
@@ -2404,7 +2402,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B58" t="s">
         <v>258</v>
@@ -2424,7 +2422,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B59" t="s">
         <v>259</v>
@@ -2444,7 +2442,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B60" t="s">
         <v>261</v>
@@ -2464,7 +2462,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B61" t="s">
         <v>260</v>
@@ -2484,7 +2482,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B62" t="s">
         <v>260</v>
@@ -2504,7 +2502,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B63" t="s">
         <v>261</v>
@@ -2524,7 +2522,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B64" t="s">
         <v>260</v>
@@ -2544,7 +2542,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B65" t="s">
         <v>260</v>
@@ -2564,7 +2562,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B66" t="s">
         <v>261</v>
@@ -2584,7 +2582,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B67" t="s">
         <v>261</v>
@@ -2604,7 +2602,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B68" t="s">
         <v>260</v>
@@ -2624,7 +2622,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B69" t="s">
         <v>260</v>
@@ -2644,7 +2642,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B70" t="s">
         <v>260</v>
@@ -2664,7 +2662,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B71" t="s">
         <v>260</v>
@@ -2684,7 +2682,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B72" t="s">
         <v>258</v>
@@ -2704,7 +2702,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B73" t="s">
         <v>261</v>
@@ -2724,7 +2722,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B74" t="s">
         <v>261</v>
@@ -2744,7 +2742,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B75" t="s">
         <v>261</v>
@@ -2764,7 +2762,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B76" t="s">
         <v>261</v>
@@ -2784,7 +2782,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B77" t="s">
         <v>260</v>
@@ -2804,7 +2802,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B78" t="s">
         <v>260</v>
@@ -2824,7 +2822,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B79" t="s">
         <v>258</v>
@@ -2844,7 +2842,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B80" t="s">
         <v>261</v>
@@ -2864,7 +2862,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B81" t="s">
         <v>260</v>
@@ -2884,7 +2882,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B82" t="s">
         <v>260</v>
@@ -2904,7 +2902,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B83" t="s">
         <v>261</v>
@@ -2924,7 +2922,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B84" t="s">
         <v>261</v>
@@ -2944,7 +2942,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B85" t="s">
         <v>261</v>
@@ -2964,7 +2962,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B86" t="s">
         <v>261</v>
@@ -2984,7 +2982,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B87" t="s">
         <v>261</v>
@@ -3004,7 +3002,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B88" t="s">
         <v>261</v>
@@ -3024,7 +3022,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B89" t="s">
         <v>258</v>
@@ -3044,7 +3042,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B90" t="s">
         <v>259</v>
@@ -3064,7 +3062,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B91" t="s">
         <v>261</v>
@@ -3084,7 +3082,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B92" t="s">
         <v>258</v>
@@ -3104,7 +3102,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B93" t="s">
         <v>259</v>
@@ -3124,7 +3122,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B94" t="s">
         <v>261</v>
@@ -3144,7 +3142,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B95" t="s">
         <v>258</v>
@@ -3164,7 +3162,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B96" t="s">
         <v>258</v>
@@ -3184,7 +3182,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B97" t="s">
         <v>257</v>
@@ -3204,7 +3202,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B98" t="s">
         <v>260</v>
@@ -3224,7 +3222,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B99" t="s">
         <v>260</v>
@@ -3244,7 +3242,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B100" t="s">
         <v>259</v>
@@ -3264,7 +3262,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B101" t="s">
         <v>258</v>
@@ -3284,7 +3282,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B102" t="s">
         <v>261</v>
@@ -3304,7 +3302,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B103" t="s">
         <v>258</v>
@@ -3324,7 +3322,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B104" t="s">
         <v>258</v>
@@ -3344,7 +3342,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B105" t="s">
         <v>260</v>
@@ -3364,7 +3362,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B106" t="s">
         <v>260</v>
@@ -3384,7 +3382,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B107" t="s">
         <v>259</v>
@@ -3404,7 +3402,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B108" t="s">
         <v>257</v>
@@ -3424,7 +3422,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B109" t="s">
         <v>261</v>
@@ -3444,7 +3442,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B110" t="s">
         <v>258</v>
@@ -3464,7 +3462,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B111" t="s">
         <v>260</v>
@@ -3484,7 +3482,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B112" t="s">
         <v>260</v>
@@ -3504,7 +3502,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B113" t="s">
         <v>257</v>
@@ -3524,7 +3522,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B114" t="s">
         <v>261</v>
@@ -3544,7 +3542,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B115" t="s">
         <v>258</v>
@@ -3564,7 +3562,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B116" t="s">
         <v>260</v>
@@ -3584,7 +3582,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B117" t="s">
         <v>260</v>
@@ -3604,7 +3602,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B118" t="s">
         <v>261</v>
@@ -3624,7 +3622,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B119" t="s">
         <v>257</v>
@@ -3644,7 +3642,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B120" t="s">
         <v>258</v>
@@ -3664,7 +3662,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B121" t="s">
         <v>260</v>
@@ -3684,7 +3682,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B122" t="s">
         <v>260</v>
@@ -3704,7 +3702,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B123" t="s">
         <v>261</v>
@@ -3724,7 +3722,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B124" t="s">
         <v>257</v>
@@ -3744,7 +3742,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B125" t="s">
         <v>258</v>
@@ -3764,7 +3762,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B126" t="s">
         <v>260</v>
@@ -3784,7 +3782,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B127" t="s">
         <v>260</v>
@@ -3804,7 +3802,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B128" t="s">
         <v>261</v>
@@ -3824,7 +3822,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B129" t="s">
         <v>257</v>
@@ -3844,7 +3842,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B130" t="s">
         <v>258</v>
@@ -3864,7 +3862,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B131" t="s">
         <v>258</v>
@@ -3884,7 +3882,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B132" t="s">
         <v>258</v>
@@ -3904,7 +3902,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B133" t="s">
         <v>258</v>
@@ -3924,7 +3922,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B134" t="s">
         <v>260</v>
@@ -3944,7 +3942,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B135" t="s">
         <v>260</v>
@@ -3964,7 +3962,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B136" t="s">
         <v>260</v>
@@ -3984,7 +3982,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B137" t="s">
         <v>260</v>
@@ -4004,7 +4002,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B138" t="s">
         <v>261</v>
@@ -4024,7 +4022,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B139" t="s">
         <v>260</v>
@@ -4044,7 +4042,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B140" t="s">
         <v>260</v>
@@ -4064,7 +4062,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B141" t="s">
         <v>261</v>
@@ -4084,7 +4082,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B142" t="s">
         <v>260</v>
@@ -4104,7 +4102,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B143" t="s">
         <v>260</v>
@@ -4124,7 +4122,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B144" t="s">
         <v>261</v>
@@ -4144,7 +4142,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B145" t="s">
         <v>258</v>
@@ -4164,7 +4162,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B146" t="s">
         <v>258</v>
@@ -4184,7 +4182,7 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B147" t="s">
         <v>261</v>
@@ -4204,7 +4202,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B148" t="s">
         <v>258</v>
@@ -4224,7 +4222,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B149" t="s">
         <v>261</v>
@@ -4244,7 +4242,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B150" t="s">
         <v>260</v>
@@ -4264,7 +4262,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B151" t="s">
         <v>260</v>
@@ -4284,7 +4282,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B152" t="s">
         <v>258</v>
@@ -4304,7 +4302,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B153" t="s">
         <v>261</v>
@@ -4324,7 +4322,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B154" t="s">
         <v>261</v>
@@ -4344,7 +4342,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B155" t="s">
         <v>261</v>
@@ -4364,7 +4362,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B156" t="s">
         <v>257</v>
@@ -4384,7 +4382,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B157" t="s">
         <v>261</v>
@@ -4404,7 +4402,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B158" t="s">
         <v>258</v>
@@ -4424,7 +4422,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B159" t="s">
         <v>260</v>
@@ -4444,7 +4442,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B160" t="s">
         <v>260</v>
@@ -4464,7 +4462,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B161" t="s">
         <v>258</v>
@@ -4484,7 +4482,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B162" t="s">
         <v>258</v>
@@ -4504,7 +4502,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B163" t="s">
         <v>258</v>
@@ -4524,7 +4522,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B164" t="s">
         <v>258</v>
@@ -4544,7 +4542,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B165" t="s">
         <v>258</v>
@@ -4564,7 +4562,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B166" t="s">
         <v>258</v>
@@ -4584,7 +4582,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B167" t="s">
         <v>258</v>
@@ -4604,7 +4602,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B168" t="s">
         <v>258</v>
@@ -4624,7 +4622,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B169" t="s">
         <v>258</v>
@@ -4644,7 +4642,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B170" t="s">
         <v>260</v>
@@ -4664,7 +4662,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B171" t="s">
         <v>260</v>
@@ -4684,7 +4682,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B172" t="s">
         <v>258</v>
@@ -4704,7 +4702,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B173" t="s">
         <v>261</v>
@@ -4724,7 +4722,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B174" t="s">
         <v>258</v>
@@ -4784,7 +4782,7 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B177" t="s">
         <v>260</v>
@@ -4804,7 +4802,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B178" t="s">
         <v>260</v>
@@ -4824,7 +4822,7 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B179" t="s">
         <v>258</v>
@@ -4844,7 +4842,7 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B180" t="s">
         <v>258</v>
@@ -4864,7 +4862,7 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B181" t="s">
         <v>260</v>
@@ -4884,7 +4882,7 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B182" t="s">
         <v>260</v>
@@ -4904,7 +4902,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B183" t="s">
         <v>261</v>
@@ -4924,7 +4922,7 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B184" t="s">
         <v>258</v>
@@ -4944,7 +4942,7 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B185" t="s">
         <v>261</v>
@@ -4964,7 +4962,7 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B186" t="s">
         <v>260</v>
@@ -4984,7 +4982,7 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B187" t="s">
         <v>260</v>
@@ -5004,7 +5002,7 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="B188" t="s">
         <v>257</v>
@@ -5024,7 +5022,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B189" t="s">
         <v>258</v>
@@ -5044,7 +5042,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B190" t="s">
         <v>261</v>
@@ -5064,7 +5062,7 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B191" t="s">
         <v>257</v>
@@ -5084,7 +5082,7 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B192" t="s">
         <v>260</v>
@@ -5104,7 +5102,7 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B193" t="s">
         <v>260</v>
@@ -5124,7 +5122,7 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B194" t="s">
         <v>257</v>
@@ -5144,7 +5142,7 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B195" t="s">
         <v>258</v>
@@ -5164,7 +5162,7 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B196" t="s">
         <v>258</v>
@@ -5184,7 +5182,7 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B197" t="s">
         <v>257</v>
@@ -5204,7 +5202,7 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B198" t="s">
         <v>258</v>
@@ -5222,7 +5220,7 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B199" t="s">
         <v>259</v>
@@ -5240,7 +5238,7 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B200" t="s">
         <v>259</v>
@@ -5258,7 +5256,7 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B201" t="s">
         <v>259</v>
@@ -5278,7 +5276,7 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B202" t="s">
         <v>259</v>
@@ -5298,7 +5296,7 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B203" t="s">
         <v>259</v>
@@ -5318,7 +5316,7 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B204" t="s">
         <v>259</v>
@@ -5338,7 +5336,7 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B205" t="s">
         <v>257</v>
@@ -5375,7 +5373,7 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B207" t="s">
         <v>257</v>
@@ -5395,7 +5393,7 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B208" t="s">
         <v>261</v>
@@ -5415,7 +5413,7 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B209" t="s">
         <v>258</v>
@@ -5435,7 +5433,7 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B210" t="s">
         <v>258</v>
@@ -5455,7 +5453,7 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B211" t="s">
         <v>257</v>
@@ -5475,7 +5473,7 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B212" t="s">
         <v>261</v>
@@ -5495,7 +5493,7 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B213" t="s">
         <v>258</v>
@@ -5515,7 +5513,7 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B214" t="s">
         <v>257</v>
@@ -5535,7 +5533,7 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B215" t="s">
         <v>261</v>
@@ -5555,7 +5553,7 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B216" t="s">
         <v>258</v>
@@ -5575,7 +5573,7 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B217" t="s">
         <v>258</v>
@@ -5595,7 +5593,7 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B218" t="s">
         <v>258</v>
@@ -5613,7 +5611,7 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B219" t="s">
         <v>258</v>
@@ -5633,7 +5631,7 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B220" t="s">
         <v>258</v>
@@ -5653,7 +5651,7 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="B221" t="s">
         <v>257</v>
@@ -5673,7 +5671,7 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B222" t="s">
         <v>258</v>
@@ -5693,7 +5691,7 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="B223" t="s">
         <v>261</v>
@@ -5712,7 +5710,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{CB690B54-ADEF-4B77-BFF1-9B7541870C3F}">
+  <autoFilter ref="A1:H223" xr:uid="{CB690B54-ADEF-4B77-BFF1-9B7541870C3F}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H223">
       <sortCondition ref="C1"/>
     </sortState>

</xml_diff>